<commit_message>
fix create inv increase
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/static/src/xlsx/template_po_nhap_khau_ver2.0.xlsx
+++ b/addons/custom/forlife_purchase/static/src/xlsx/template_po_nhap_khau_ver2.0.xlsx
@@ -1,33 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Zalo Received Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aht\Desktop\Forlife\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBCF229-2814-4FB3-AF02-7B4F73992AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="PO - HH" sheetId="2" r:id="rId1"/>
     <sheet name="PO - DV" sheetId="3" r:id="rId2"/>
     <sheet name="PO - TS" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{3DFAA85E-FFBF-4895-AB90-889BB0014873}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{38E52348-2636-46CD-A498-4287AC79F31E}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{1FB802E4-E7BE-4F7D-B839-B3943951D3EE}">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,12 +109,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{AB0808F2-072A-45A5-BDBD-BA3B2823F000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{DD18E7C6-EF0B-43DA-8B08-B97DB19FD8E1}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{86C555A5-BB69-4674-94D0-8285D72B7F76}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -194,12 +193,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{A9046A09-F780-4F39-96CA-C0E4EA3C8A40}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{0078464F-986D-4B88-BE5C-5FDBABA238DD}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -247,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{AC791F5E-4D01-4100-93D7-4D2F24A3ADE3}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -278,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
   <si>
     <t>Hàng hóa</t>
   </si>
@@ -307,9 +306,6 @@
     <t>Chi tiết đơn hàng / Hàng tặng</t>
   </si>
   <si>
-    <t>Chi tiết đơn hàng / Thuế(%)</t>
-  </si>
-  <si>
     <t>Chi tiết đơn hàng / Chiết khấu(%)</t>
   </si>
   <si>
@@ -368,7 +364,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -378,7 +374,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -393,7 +389,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -403,7 +399,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -418,7 +414,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -428,7 +424,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -443,7 +439,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -453,7 +449,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -468,7 +464,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -478,7 +474,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -493,7 +489,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -503,7 +499,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -518,7 +514,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -528,7 +524,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -543,7 +539,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -553,7 +549,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -568,7 +564,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -578,7 +574,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -593,7 +589,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -603,7 +599,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -620,7 +616,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -631,7 +627,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -641,7 +637,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -656,7 +652,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -666,7 +662,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -685,7 +681,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -695,7 +691,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -728,7 +724,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -738,7 +734,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -753,7 +749,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -764,7 +760,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -774,7 +770,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -802,7 +798,7 @@
         <i/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -812,7 +808,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -827,7 +823,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -837,7 +833,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -852,7 +848,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -862,7 +858,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -877,7 +873,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -887,7 +883,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -901,37 +897,37 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -952,28 +948,28 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -1002,7 +998,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -1066,7 +1062,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1077,7 +1073,7 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1091,12 +1087,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="Tiền tệ" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1428,80 +1424,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL8" sqref="AL8"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.19921875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.19921875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.3984375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="33.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.09765625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="36.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="39.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30" style="1" customWidth="1"/>
-    <col min="23" max="23" width="28.09765625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="31.19921875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="30.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="42" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="32.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="37.19921875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="36.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="29.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="22.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="8.8984375" style="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30" style="1" customWidth="1"/>
+    <col min="22" max="22" width="28.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="31.140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="42" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="37.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="39" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>2</v>
@@ -1516,25 +1511,25 @@
         <v>3</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="S1" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>9</v>
@@ -1543,43 +1538,43 @@
         <v>10</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="X1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG1" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH1" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="AI1" s="11" t="s">
         <v>13</v>
@@ -1590,19 +1585,16 @@
       <c r="AK1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AL1" s="11" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:38" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1620,7 +1612,7 @@
         <v>45133</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1" t="b">
         <v>0</v>
@@ -1629,10 +1621,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="N2" s="1" t="b">
         <v>0</v>
@@ -1641,7 +1633,7 @@
         <v>20</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q2" s="14">
         <v>1</v>
@@ -1650,64 +1642,64 @@
         <v>10</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="1">
+        <v>16</v>
+      </c>
+      <c r="T2" s="1">
         <v>2</v>
       </c>
+      <c r="U2" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="V2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="W2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="17" t="s">
+      <c r="W2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>200</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>50</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="AG2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>23960</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>50</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1198000</v>
+      </c>
+      <c r="AK2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="Z2" s="1">
-        <v>200</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>5</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>4</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>50</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>23960</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>50</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>1198000</v>
-      </c>
-      <c r="AL2" s="1" t="b">
-        <v>1</v>
-      </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
   </sheetData>
@@ -1719,75 +1711,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" customWidth="1"/>
-    <col min="3" max="3" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.69921875" customWidth="1"/>
-    <col min="13" max="13" width="24.796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.09765625" customWidth="1"/>
-    <col min="16" max="16" width="25.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.3984375" customWidth="1"/>
-    <col min="19" max="19" width="25.09765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.69921875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.69921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.8984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="33.3984375" customWidth="1"/>
-    <col min="25" max="25" width="42.59765625" customWidth="1"/>
-    <col min="26" max="26" width="38.3984375" customWidth="1"/>
-    <col min="27" max="27" width="44.8984375" customWidth="1"/>
-    <col min="28" max="28" width="33.796875" customWidth="1"/>
-    <col min="29" max="29" width="40.3984375" customWidth="1"/>
-    <col min="30" max="30" width="20.3984375" customWidth="1"/>
-    <col min="31" max="31" width="19" customWidth="1"/>
-    <col min="32" max="32" width="17.796875" customWidth="1"/>
-    <col min="33" max="33" width="23.3984375" customWidth="1"/>
-    <col min="34" max="35" width="22.3984375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.140625" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.42578125" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.42578125" customWidth="1"/>
+    <col min="24" max="24" width="42.5703125" customWidth="1"/>
+    <col min="25" max="25" width="38.42578125" customWidth="1"/>
+    <col min="26" max="26" width="44.85546875" customWidth="1"/>
+    <col min="27" max="27" width="33.85546875" customWidth="1"/>
+    <col min="28" max="28" width="40.42578125" customWidth="1"/>
+    <col min="29" max="29" width="20.42578125" customWidth="1"/>
+    <col min="30" max="30" width="19" customWidth="1"/>
+    <col min="31" max="31" width="17.85546875" customWidth="1"/>
+    <col min="32" max="32" width="23.42578125" customWidth="1"/>
+    <col min="33" max="34" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>7</v>
@@ -1799,51 +1790,48 @@
         <v>3</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>50</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1867,10 +1855,10 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>0</v>
@@ -1879,21 +1867,21 @@
         <v>20</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P2" s="14">
         <v>1</v>
       </c>
-      <c r="R2" s="1">
+      <c r="Q2" s="1">
         <v>10</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="W2" s="1">
+      <c r="U2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1901,8 +1889,8 @@
   <conditionalFormatting sqref="L2:N2">
     <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:U2">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  <conditionalFormatting sqref="O2:T2">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1911,77 +1899,76 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AJ3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.09765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.69921875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.69921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.8984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="42" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="42.296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="36.796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="39.19921875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.09765625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.09765625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.8984375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="42" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="39" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>7</v>
@@ -1993,67 +1980,67 @@
         <v>3</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>50</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF1" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE1" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="AG1" s="11" t="s">
         <v>13</v>
@@ -2064,19 +2051,16 @@
       <c r="AI1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AJ1" s="11" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -2100,10 +2084,10 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>0</v>
@@ -2112,28 +2096,27 @@
         <v>20</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P2" s="14">
         <v>10001</v>
       </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1">
+      <c r="Q2" s="1">
         <v>10</v>
       </c>
+      <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="W2" s="1">
+      <c r="U2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2273,18 +2256,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2306,6 +2289,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40835504-4F46-4A81-BD00-C7B4354D2E50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53ADD2F5-A402-45D1-88A3-5F6CA6334DE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2319,12 +2310,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40835504-4F46-4A81-BD00-C7B4354D2E50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>